<commit_message>
oncogenes now does driver and target
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
   <si>
     <t>Column</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>failing hard</t>
+  </si>
+  <si>
+    <t>oncogenes</t>
+  </si>
+  <si>
+    <t>db troubles</t>
   </si>
 </sst>
 </file>
@@ -594,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48:E56"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,6 +907,15 @@
       <c r="B37" t="s">
         <v>35</v>
       </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -908,6 +923,15 @@
       </c>
       <c r="B38" t="s">
         <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>